<commit_message>
add: PO field for pdf,excel template product requisition form
</commit_message>
<xml_diff>
--- a/app/backend/public/templates/excel/product-requisition-form.xlsx
+++ b/app/backend/public/templates/excel/product-requisition-form.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F9209A-3DB5-41CB-8E3E-027C6AC3B3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>PHIẾU YÊU CẦU
 VẬT TƯ</t>
@@ -65,12 +66,15 @@
   </si>
   <si>
     <t>GHI CHÚ</t>
+  </si>
+  <si>
+    <t>PO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -531,25 +535,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="49.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="6" max="6" width="19.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
       <c r="C1" s="8" t="s">
@@ -563,7 +567,7 @@
       </c>
       <c r="F1" s="14"/>
     </row>
-    <row r="2" spans="1:6" ht="60.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
       <c r="C2" s="8"/>
@@ -575,7 +579,7 @@
       </c>
       <c r="F2" s="14"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -586,7 +590,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -597,7 +601,14 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="9" spans="1:6" s="6" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="9" spans="1:6" s="6" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -617,7 +628,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -625,7 +636,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -633,7 +644,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -641,7 +652,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -649,7 +660,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -657,7 +668,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -665,7 +676,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -673,7 +684,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -681,7 +692,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -689,7 +700,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -697,7 +708,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -705,7 +716,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -713,7 +724,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -721,7 +732,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -729,7 +740,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -737,7 +748,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -745,7 +756,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -753,7 +764,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -761,7 +772,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -769,7 +780,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -777,7 +788,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -785,7 +796,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -793,7 +804,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -801,7 +812,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -809,7 +820,7 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -817,7 +828,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -825,7 +836,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -833,7 +844,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -841,7 +852,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -849,7 +860,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -857,7 +868,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -865,7 +876,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -873,7 +884,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -881,7 +892,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -889,7 +900,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -897,7 +908,7 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -905,7 +916,7 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -913,7 +924,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -921,7 +932,7 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -929,7 +940,7 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -937,7 +948,7 @@
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -945,7 +956,7 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -953,7 +964,7 @@
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -961,7 +972,7 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -969,7 +980,7 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -977,7 +988,7 @@
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -985,7 +996,7 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -993,7 +1004,7 @@
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1001,7 +1012,7 @@
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1009,7 +1020,7 @@
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -1017,7 +1028,7 @@
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -1025,7 +1036,7 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1033,7 +1044,7 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -1041,7 +1052,7 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -1049,7 +1060,7 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -1057,7 +1068,7 @@
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -1065,7 +1076,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -1074,7 +1085,8 @@
       <c r="F66" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="E7:F7"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="C1:C2"/>

</xml_diff>